<commit_message>
commeting done; todo: rubrics
</commit_message>
<xml_diff>
--- a/tests/partial.xlsx
+++ b/tests/partial.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -126,7 +126,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">Sat Dec 22 12:06:10 UTC 2018 | 4951</t>
+  </si>
   <si>
     <t xml:space="preserve">Age</t>
   </si>
@@ -157,7 +160,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -179,6 +182,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -295,28 +304,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -324,7 +337,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,7 +417,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -436,6 +449,12 @@
         </c:rich>
       </c:tx>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -520,11 +539,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="81412329"/>
-        <c:axId val="20472844"/>
+        <c:axId val="14083835"/>
+        <c:axId val="52836962"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81412329"/>
+        <c:axId val="14083835"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,6 +576,12 @@
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
@@ -583,14 +608,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20472844"/>
+        <c:crossAx val="52836962"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20472844"/>
+        <c:axId val="52836962"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,6 +657,12 @@
             </c:rich>
           </c:tx>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
@@ -658,7 +689,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81412329"/>
+        <c:crossAx val="14083835"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -712,13 +743,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>102960</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>321120</xdr:colOff>
+      <xdr:colOff>320040</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -727,8 +758,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2905560" y="830520"/>
-          <a:ext cx="980280" cy="27720"/>
+          <a:off x="2905560" y="822960"/>
+          <a:ext cx="979200" cy="27000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -774,13 +805,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>312480</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>599040</xdr:colOff>
+      <xdr:colOff>598320</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>111240</xdr:rowOff>
+      <xdr:rowOff>110880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -789,8 +820,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3877200" y="556200"/>
-          <a:ext cx="1048680" cy="652320"/>
+          <a:off x="3877200" y="548640"/>
+          <a:ext cx="1047960" cy="651600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -826,7 +857,7 @@
             <a:t>This is a </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-            <a:latin typeface="나눔고딕"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -845,7 +876,7 @@
             <a:t>column cell </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-            <a:latin typeface="나눔고딕"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -864,7 +895,7 @@
             <a:t>Formula Block</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-            <a:latin typeface="나눔고딕"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -873,16 +904,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>57960</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>783720</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>352440</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:colOff>57240</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -891,8 +922,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="2860560" y="2275560"/>
-          <a:ext cx="294480" cy="271440"/>
+          <a:off x="2566080" y="1996200"/>
+          <a:ext cx="293760" cy="270720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -936,15 +967,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>83880</xdr:colOff>
+      <xdr:colOff>84240</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:rowOff>15480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>370440</xdr:colOff>
+      <xdr:colOff>369720</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>118800</xdr:rowOff>
+      <xdr:rowOff>118440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -953,8 +984,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2886480" y="2575440"/>
-          <a:ext cx="1048680" cy="652320"/>
+          <a:off x="2886840" y="2567880"/>
+          <a:ext cx="1047600" cy="651600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -990,7 +1021,7 @@
             <a:t>This is a </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-            <a:latin typeface="나눔고딕"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -1009,7 +1040,7 @@
             <a:t>row cell </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-            <a:latin typeface="나눔고딕"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -1028,7 +1059,7 @@
             <a:t>Formula Block</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-            <a:latin typeface="나눔고딕"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -1037,16 +1068,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>385920</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>456840</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>60840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>314640</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>39960</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>384840</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1055,8 +1086,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="8522640" y="1147680"/>
-          <a:ext cx="690840" cy="355320"/>
+          <a:off x="7831440" y="784440"/>
+          <a:ext cx="690120" cy="354600"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1102,13 +1133,13 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>464760</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>362880</xdr:colOff>
+      <xdr:colOff>362520</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>19800</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1117,8 +1148,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8601480" y="1562040"/>
-          <a:ext cx="1422000" cy="652320"/>
+          <a:off x="8601480" y="1554480"/>
+          <a:ext cx="1421640" cy="651600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1154,7 +1185,7 @@
             <a:t>This is a </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-            <a:latin typeface="나눔고딕"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -1173,7 +1204,7 @@
             <a:t>row+column cell </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-            <a:latin typeface="나눔고딕"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
         <a:p>
@@ -1192,7 +1223,7 @@
             <a:t>Formula Block</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
-            <a:latin typeface="나눔고딕"/>
+            <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -1204,13 +1235,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>501840</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>119160</xdr:rowOff>
+      <xdr:rowOff>119520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>669240</xdr:colOff>
+      <xdr:colOff>668880</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:rowOff>4320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1218,8 +1249,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2284200" y="3411000"/>
-        <a:ext cx="5759640" cy="3322440"/>
+        <a:off x="2284200" y="3403440"/>
+        <a:ext cx="5759280" cy="3321720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1239,8 +1270,8 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1251,27 +1282,30 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="9.01"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>1</v>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>2</v>
@@ -1296,30 +1330,30 @@
       <c r="B3" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="4" t="n">
         <f aca="false">B3/A3</f>
         <v>3</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="4" t="n">
         <f aca="false">$H3/I$2</f>
         <v>2.5</v>
       </c>
-      <c r="J3" s="3" t="n">
+      <c r="J3" s="4" t="n">
         <f aca="false">$H3/J$2</f>
         <v>1.25</v>
       </c>
-      <c r="K3" s="3" t="n">
+      <c r="K3" s="4" t="n">
         <f aca="false">$H3/K$2</f>
         <v>0.833333333333333</v>
       </c>
-      <c r="L3" s="3" t="n">
+      <c r="L3" s="4" t="n">
         <f aca="false">$H3/L$2</f>
         <v>0.625</v>
       </c>
-      <c r="M3" s="3" t="n">
+      <c r="M3" s="4" t="n">
         <f aca="false">$H3/M$2</f>
         <v>0.5</v>
       </c>
@@ -1331,30 +1365,30 @@
       <c r="B4" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="4" t="n">
         <f aca="false">B4/A4</f>
         <v>2.33333333333333</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="4" t="n">
         <f aca="false">$H4/I$2</f>
         <v>5</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="4" t="n">
         <f aca="false">$H4/J$2</f>
         <v>2.5</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="K4" s="4" t="n">
         <f aca="false">$H4/K$2</f>
         <v>1.66666666666667</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="L4" s="4" t="n">
         <f aca="false">$H4/L$2</f>
         <v>1.25</v>
       </c>
-      <c r="M4" s="3" t="n">
+      <c r="M4" s="4" t="n">
         <f aca="false">$H4/M$2</f>
         <v>1</v>
       </c>
@@ -1366,30 +1400,30 @@
       <c r="B5" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="4" t="n">
         <f aca="false">B5/A5</f>
         <v>2</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="I5" s="4" t="n">
         <f aca="false">$H5/I$2</f>
         <v>7.5</v>
       </c>
-      <c r="J5" s="3" t="n">
+      <c r="J5" s="4" t="n">
         <f aca="false">$H5/J$2</f>
         <v>3.75</v>
       </c>
-      <c r="K5" s="3" t="n">
+      <c r="K5" s="4" t="n">
         <f aca="false">$H5/K$2</f>
         <v>2.5</v>
       </c>
-      <c r="L5" s="3" t="n">
+      <c r="L5" s="4" t="n">
         <f aca="false">$H5/L$2</f>
         <v>1.875</v>
       </c>
-      <c r="M5" s="3" t="n">
+      <c r="M5" s="4" t="n">
         <f aca="false">$H5/M$2</f>
         <v>1.5</v>
       </c>
@@ -1401,30 +1435,30 @@
       <c r="B6" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="4" t="n">
         <f aca="false">B6/A6</f>
         <v>2.08333333333333</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="4" t="n">
         <f aca="false">$H6/I$2</f>
         <v>10</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="J6" s="4" t="n">
         <f aca="false">$H6/J$2</f>
         <v>5</v>
       </c>
-      <c r="K6" s="3" t="n">
+      <c r="K6" s="4" t="n">
         <f aca="false">$H6/K$2</f>
         <v>3.33333333333333</v>
       </c>
-      <c r="L6" s="3" t="n">
+      <c r="L6" s="4" t="n">
         <f aca="false">$H6/L$2</f>
         <v>2.5</v>
       </c>
-      <c r="M6" s="3" t="n">
+      <c r="M6" s="4" t="n">
         <f aca="false">$H6/M$2</f>
         <v>2</v>
       </c>
@@ -1436,218 +1470,218 @@
       <c r="B7" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="4" t="n">
         <f aca="false">B7/A7</f>
         <v>1.83333333333333</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="4" t="n">
+      <c r="A10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="n">
+      <c r="C10" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="D10" s="4" t="n">
+      <c r="D10" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="E10" s="5" t="n">
         <v>24</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F10" s="5" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="4" t="n">
+      <c r="A11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="C11" s="4" t="n">
+      <c r="C11" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="D11" s="4" t="n">
+      <c r="D11" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="E11" s="5" t="n">
         <v>50</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F11" s="5" t="n">
         <v>55</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="5" t="n">
+      <c r="A12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="6" t="n">
         <f aca="false">B11/B10</f>
         <v>3</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="6" t="n">
         <f aca="false">C11/C10</f>
         <v>2.33333333333333</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="D12" s="6" t="n">
         <f aca="false">D11/D10</f>
         <v>2</v>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" s="6" t="n">
         <f aca="false">E11/E10</f>
         <v>2.08333333333333</v>
       </c>
-      <c r="F12" s="5" t="n">
+      <c r="F12" s="6" t="n">
         <f aca="false">F11/F10</f>
         <v>1.83333333333333</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L15" s="6"/>
+      <c r="L15" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
-        <v>3</v>
+      <c r="A23" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
-        <v>4</v>
+      <c r="A24" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="7" t="n">
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="8" t="n">
         <f aca="false">F10+F11</f>
         <v>85</v>
       </c>
-      <c r="N24" s="6"/>
+      <c r="N24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
-        <v>5</v>
+      <c r="A25" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
-        <v>6</v>
+      <c r="A26" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1670,10 +1704,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C13:J36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1681,245 +1715,250 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.57"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>